<commit_message>
New Questionnaires Uploaded, Feedback Collated
Updated the excel doc, plus uploaded new questionnaires. Single player questionnaires are currently not included in the results
</commit_message>
<xml_diff>
--- a/Elliot/Feedback/FeedbackCollation.xlsx
+++ b/Elliot/Feedback/FeedbackCollation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Games\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eternallyrekt\Documents\GitHub\level-6-stuck-in-a-lift-studios-1\Elliot\Feedback\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -71,9 +71,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,12 +105,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,7 +411,7 @@
   <dimension ref="B2:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,119 +420,135 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
         <v>2</v>
       </c>
-      <c r="C4">
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>